<commit_message>
int형인 phone을 String으로 바꿈.
</commit_message>
<xml_diff>
--- a/DB sql query/DB 현황.xlsx
+++ b/DB sql query/DB 현황.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="9795"/>
@@ -14,12 +14,586 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="165">
   <si>
     <t>String</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chkIn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chkOut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookingNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Booking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mileage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mileage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myCamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>startDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campOwner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campAddr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campPost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campPerson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campToilet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campShower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campElect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campSiteName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campSiteStock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campCaravan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campGlamping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campPlayground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campFood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sellerId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>siteId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>startBusyDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endBusyDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>busyDayPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>busyWkndPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dayPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wkndPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SellerRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>joinDate</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>statusType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk/ai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sellerId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk / ai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BookedSite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leaveMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>1.결제완료 2.결제 취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancelDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookedSiteNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stayDay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardOne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>writer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>writeDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk / ai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = 캠핑장 공지사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = 캠핑장 정책사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardTwo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qtype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = 예약 / 취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = 결제 / 환불</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 = 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = 캠핑장 Q&amp;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardTwoRe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>originNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupOrd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parentNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campReview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 = 고객센터 공지사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 = 고객센터 FAQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = 고객센터 Q&amp;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>campPhone</t>
+  </si>
+  <si>
+    <t>campOwner</t>
+  </si>
+  <si>
+    <t>campAddr</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>stopDate</t>
+  </si>
+  <si>
+    <t>sellerId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two.no/FK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>pw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -40,614 +614,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>joinDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>userId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>chkIn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chkOut</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bookingNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">int </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Member</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Booking</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
+    <t>businessNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessAddr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>businessPost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sellerId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>joinDate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mileage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mileage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>myCamp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>startDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>endDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campOwner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>businessNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campAddr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campPost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campPerson</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campToilet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campShower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campElect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Seller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campSiteName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campSiteStock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campCaravan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campGlamping</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campPlayground</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campFood</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sellerId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>siteId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">int </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Site</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>startBusyDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>endBusyDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>busyDayPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>busyWkndPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dayPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">String </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wkndPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sellerId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SellerRequest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>joinDate</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>statusType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>businessName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>joinDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pk/ai</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sellerId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pk / ai</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BookedSite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l_member</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l_Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>leaveMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>1.결제완료 2.결제 취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cancelDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>`</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>picture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bookedSiteNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stayDay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardOne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>writer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dateTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>writeDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pk / ai</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2000자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 = 캠핑장 공지사항</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 = 캠핑장 정책사항</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardTwo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qtype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 = 예약 / 취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 = 결제 / 환불</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 = 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 = 캠핑장 Q&amp;A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardTwoRe</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>originNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupOrd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parentNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campReview</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 = 고객센터 공지사항</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 = 고객센터 FAQ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 = 고객센터 Q&amp;A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>businessPhone</t>
-  </si>
-  <si>
-    <t>businessEmail</t>
-  </si>
-  <si>
-    <t>businessPost</t>
-  </si>
-  <si>
-    <t>campPhone</t>
-  </si>
-  <si>
-    <t>campOwner</t>
-  </si>
-  <si>
-    <t>campAddr</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>stopDate</t>
-  </si>
-  <si>
-    <t>businessAddr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sellerId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>double</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>longitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Two.no/FK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1004,9 +1027,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,6 +1070,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,6 +1123,11 @@
       <color rgb="FF0099CC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1178,6 +1206,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1212,6 +1241,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1387,14 +1417,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -1407,394 +1437,394 @@
     <col min="17" max="17" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="34"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="33"/>
       <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="35"/>
+      <c r="D1" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="34"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="36"/>
+      <c r="G1" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="35"/>
       <c r="I1" s="8">
         <v>1</v>
       </c>
-      <c r="J1" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="K1" s="41"/>
+      <c r="J1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="40"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="33"/>
+      <c r="M1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="32"/>
       <c r="O1" s="3">
         <v>1</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I6" s="8"/>
       <c r="M6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="K8" s="45"/>
+      <c r="J8" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="44"/>
       <c r="L8" s="8">
         <v>1</v>
       </c>
-      <c r="M8" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="44"/>
+      <c r="M8" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="43"/>
       <c r="O8" s="3">
         <v>1</v>
       </c>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
       <c r="I9" s="14"/>
       <c r="J9" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="14"/>
       <c r="J10" s="25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="12"/>
@@ -1803,26 +1833,26 @@
         <v>0</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="13"/>
@@ -1832,14 +1862,14 @@
         <v>0</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G13" s="27"/>
       <c r="H13" s="28"/>
       <c r="I13" s="29"/>
@@ -1847,805 +1877,802 @@
       <c r="K13" s="3"/>
       <c r="L13" s="5"/>
       <c r="Q13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="37"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="36"/>
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="37"/>
+      <c r="D14" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="36"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="38"/>
+      <c r="G14" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="37"/>
       <c r="I14" s="25">
         <v>1</v>
       </c>
-      <c r="J14" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="40"/>
+      <c r="J14" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="39"/>
       <c r="L14" s="3">
         <v>1</v>
       </c>
-      <c r="M14" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="N14" s="43"/>
+      <c r="M14" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" s="42"/>
       <c r="O14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="25" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I16" s="25"/>
       <c r="J16" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="20" t="s">
-        <v>97</v>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>164</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="25" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="25" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="I23" s="25"/>
       <c r="J23" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="4"/>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
       <c r="G24" s="2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
       <c r="G25" s="2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J26" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="30"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="45"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="30"/>
+      <c r="D27" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="45"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="30"/>
+      <c r="G27" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="45"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="K27" s="30"/>
+      <c r="J27" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="K27" s="45"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="25" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I32" s="8"/>
       <c r="J32" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="D35" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="19"/>
       <c r="G36" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D42" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D43" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D44" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="J8:K8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="G27:H27"/>
@@ -2662,6 +2689,9 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>